<commit_message>
Fixed a number of errors that were preventing the app from running. Added a couple of ammendments to the final prepared template to align with expected format. Added addiitonal R packages to database.
</commit_message>
<xml_diff>
--- a/inst/IPPO_app/App_backend/records.xlsx
+++ b/inst/IPPO_app/App_backend/records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://curtin-my.sharepoint.com/personal/299755c_curtin_edu_au/Documents/Documents/GitHub/rippo/inst/IPPO_app/App_backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{F8FEE642-38FC-49F6-97FC-CC06C7085F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BD3B8C3-BBEB-4134-A5F5-29CB26B968A5}"/>
+  <xr:revisionPtr revIDLastSave="257" documentId="13_ncr:1_{F8FEE642-38FC-49F6-97FC-CC06C7085F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4D2F8E2-6F02-415A-9593-EBC1C3BFF816}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-9165" windowWidth="21840" windowHeight="37920" xr2:uid="{479BC5EC-0D1D-48AC-8D25-FBC6E8C102EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="288">
   <si>
     <t>Jeff Bezanson, Stefan Karpinski, Viral B. Shah, and other contributors. See: https://github.com/JuliaLang/julia/contributors</t>
   </si>
@@ -822,6 +822,135 @@
   </si>
   <si>
     <t>Quarto R Interface</t>
+  </si>
+  <si>
+    <t>openxlsx</t>
+  </si>
+  <si>
+    <t>Philipp Schauberger [aut], Alexander Walker [aut], Luca Braglia [ctb], Joshua Sturm [ctb], Jan Marvin Garbuszus [ctb, cre], Jordan Mark Barbone [ctb], David Zimmermann [ctb], Reinhold Kainhofer [ctb]</t>
+  </si>
+  <si>
+    <t>{openxlsx} Simplifies the creation of Excel .xlsx files by providing a high level interface to writing, styling and editing worksheets. Through the use of 'Rcpp', read/write times are comparable to the 'xlsx' and 'XLConnect' packages with the added benefit of removing the dependency on Java.</t>
+  </si>
+  <si>
+    <t>{openxlsx} is made freely available for use and redistribution under the MIT Licence.</t>
+  </si>
+  <si>
+    <t>Eike Luedeling ORCID iD [aut, cre], Lars Caspersen ORCID iD [aut], Eduardo Fernandez ORCID iD [aut]</t>
+  </si>
+  <si>
+    <t>chillR</t>
+  </si>
+  <si>
+    <t>{chillR} is made freely available for use and redistribution under the GPL-3 Licence. </t>
+  </si>
+  <si>
+    <t>janitor</t>
+  </si>
+  <si>
+    <t>Sam Firke [aut, cre], Bill Denney [ctb], Chris Haid [ctb], Ryan Knight [ctb], Malte Grosser [ctb], Jonathan Zadra [ctb]</t>
+  </si>
+  <si>
+    <t>forcats</t>
+  </si>
+  <si>
+    <t>{forcats} Helpers for reordering factor levels (including moving specified levels to front, ordering by first appearance, reversing, and randomly shuffling), and tools for modifying factor levels (including collapsing rare levels into other, 'anonymising', and manually 'recoding').</t>
+  </si>
+  <si>
+    <t>{janitor} The main janitor functions can: perfectly format data.frame column names; provide quick counts of variable combinations (i.e., frequency tables and crosstabs); and explore duplicate records. Other janitor functions nicely format the tabulation results. These tabulate-and-report functions approximate popular features of SPSS and Microsoft Excel. This package follows the principles of the "tidyverse" and works well with the pipe function %&gt;%. janitor was built with beginning-to-intermediate R users in mind and is optimized for user-friendliness.</t>
+  </si>
+  <si>
+    <t>{chillR} The phenology of plants (i.e. the timing of their annual life phases) depends on climatic cues. For temperate trees and many other plants, spring phases, such as leaf emergence and flowering, have been found to result from the effects of both cool (chilling) conditions and heat. Fruit tree scientists (pomologists) have developed some metrics to quantify chilling and heat (e.g. see Luedeling (2012) &lt;doi:10.1016/j.scienta.2012.07.011&gt;). 'chillR' contains functions for processing temperature records into chilling (Chilling Hours, Utah Chill Units and Chill Portions) and heat units (Growing Degree Hours). Regarding chilling metrics, Chill Portions are often considered the most promising, but they are difficult to calculate. This package makes it easy. 'chillR' also contains procedures for conducting a PLS analysis relating phenological dates (e.g. bloom dates) to either mean temperatures or mean chill and heat accumulation rates, based on long-term weather and phenology records (Luedeling and Gassner (2012) &lt;doi:10.1016/j.agrformet.2011.10.020&gt;). As of version 0.65, it also includes functions for generating weather scenarios with a weather generator, for conducting climate change analyses for temperature-based climatic metrics and for plotting results from such analyses. Since version 0.70, 'chillR' contains a function for interpolating hourly temperature records.</t>
+  </si>
+  <si>
+    <t>lubridate</t>
+  </si>
+  <si>
+    <t>{lubridate} Functions to work with date-times and time-spans: fast and user friendly parsing of date-time data, extraction and updating of components of a date-time (years, months, days, hours, minutes, and seconds), algebraic manipulation on date-time and time-span objects. The 'lubridate' package has a consistent and memorable syntax that makes working with dates easy and fun.</t>
+  </si>
+  <si>
+    <t>Vitalie Spinu [aut, cre], Garrett Grolemund [aut], Hadley Wickham [aut], Davis Vaughan [ctb], Ian Lyttle [ctb], Imanuel Costigan [ctb], Jason Law [ctb], Doug Mitarotonda [ctb], Joseph Larmarange [ctb], Jonathan Boiser [ctb], Chel Hee Lee [ctb]</t>
+  </si>
+  <si>
+    <t>purrr</t>
+  </si>
+  <si>
+    <t>{purrr} A complete and consistent functional programming toolkit for R.</t>
+  </si>
+  <si>
+    <t>Hadley Wickham ORCID iD [aut, cre], Lionel Henry [aut], Posit Software, PBC [cph, fnd]</t>
+  </si>
+  <si>
+    <t>{tidyr} Tools to help to create tidy data, where each column is a variable, each row is an observation, and each cell contains a single value. 'tidyr' contains tools for changing the shape (pivoting) and hierarchy (nesting and 'unnesting') of a dataset, turning deeply nested lists into rectangular data frames ('rectangling'), and extracting values out of string columns. It also includes tools for working with missing values (both implicit and explicit).</t>
+  </si>
+  <si>
+    <t>tidyr</t>
+  </si>
+  <si>
+    <t>Hadley Wickham [aut, cre], Davis Vaughan [aut], Maximilian Girlich [aut], Kevin Ushey [ctb], Posit Software, PBC [cph, fnd]</t>
+  </si>
+  <si>
+    <t>{brms} Fit Bayesian generalized (non-)linear multivariate multilevel models using 'Stan' for full Bayesian inference. A wide range of distributions and link functions are supported, allowing users to fit – among others – linear, robust linear, count data, survival, response times, ordinal, zero-inflated, hurdle, and even self-defined mixture models all in a multilevel context. Further modeling options include both theory-driven and data-driven non-linear terms, auto-correlation structures, censoring and truncation, meta-analytic standard errors, and quite a few more. In addition, all parameters of the response distribution can be predicted in order to perform distributional regression. Prior specifications are flexible and explicitly encourage users to apply prior distributions that actually reflect their prior knowledge. Models can easily be evaluated and compared using several methods assessing posterior or prior predictions.</t>
+  </si>
+  <si>
+    <t>Paul-Christian Bürkner [aut, cre], Jonah Gabry [ctb], Sebastian Weber [ctb], Andrew Johnson [ctb], Martin Modrak [ctb], Hamada S. Badr [ctb], Frank Weber [ctb], Aki Vehtari [ctb], Mattan S. Ben-Shachar [ctb], Hayden Rabel [ctb], Simon C. Mills [ctb], Stephen Wild [ctb], Ven Popov [ctb]</t>
+  </si>
+  <si>
+    <t>brms</t>
+  </si>
+  <si>
+    <t>{fda} These functions were developed to support functional data analysis as described in Ramsay, J. O. and Silverman, B. W. (2005) Functional Data Analysis. New York: Springer and in Ramsay, J. O., Hooker, Giles, and Graves, Spencer (2009). Functional Data Analysis with R and Matlab (Springer). The package includes data sets and script files working many examples including all but one of the 76 figures in this latter book.</t>
+  </si>
+  <si>
+    <t>James Ramsay [aut, cre], Giles Hooker [ctb], Spencer Graves [ctb]</t>
+  </si>
+  <si>
+    <t>fda</t>
+  </si>
+  <si>
+    <t>{targets} Pipeline tools coordinate the pieces of computationally demanding analysis projects. The 'targets' package is a 'Make'-like pipeline tool for statistics and data science in R. The package skips costly runtime for tasks that are already up to date, orchestrates the necessary computation with implicit parallel computing, and abstracts files as R objects. If all the current output matches the current upstream code and data, then the whole pipeline is up to date, and the results are more trustworthy than otherwise. The methodology in this package borrows from GNU 'Make' (2015, ISBN:978-9881443519) and 'drake' (2018, &lt;doi:10.21105/joss.00550&gt;).</t>
+  </si>
+  <si>
+    <t>William Michael Landau ORCID iD [aut, cre], Matthew T. Warkentin [ctb], Mark Edmondson ORCID iD [ctb], Samantha Oliver ORCID iD [rev], Tristan Mahr ORCID iD [rev], Eli Lilly and Company [cph, fnd]</t>
+  </si>
+  <si>
+    <t>targets</t>
+  </si>
+  <si>
+    <t>Baptiste Auguie [aut, cre], Anton Antonov [ctb]</t>
+  </si>
+  <si>
+    <t>{gridExtra} Provides a number of user-level functions to work with "grid" graphics, notably to arrange multiple grid-based plots on a page, and draw tables.</t>
+  </si>
+  <si>
+    <t>gridExtra</t>
+  </si>
+  <si>
+    <t>{lubridate} is made freely available for use and redistribution under the GPL-3 Licence. </t>
+  </si>
+  <si>
+    <t>{brms} is made freely available for use and redistribution under the GPL-2 Licence. </t>
+  </si>
+  <si>
+    <t>{targets} is made freely available for use and redistribution under the MIT Licence.</t>
+  </si>
+  <si>
+    <t>{fda} is made freely available for use and redistribution under the GPL-3 Licence. </t>
+  </si>
+  <si>
+    <t>{gridExtra} is made freely available for use and redistribution under the GPL-3 Licence. </t>
+  </si>
+  <si>
+    <t>{janitor} is made freely available for use and redistribution under the MIT Licence.</t>
+  </si>
+  <si>
+    <t>{forcats} is made freely available for use and redistribution under the MIT Licence.</t>
+  </si>
+  <si>
+    <t>{purrr} is made freely available for use and redistribution under the MIT Licence.</t>
+  </si>
+  <si>
+    <t>{tidyr} is made freely available for use and redistribution under the MIT Licence.</t>
   </si>
 </sst>
 </file>
@@ -978,10 +1107,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1301,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC887BEF-120E-4512-A19E-0B1FB7E9F907}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="E40" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3079,8 +3204,361 @@
         <v>184</v>
       </c>
     </row>
+    <row r="56" spans="1:10" ht="90">
+      <c r="A56" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B56" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C56" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="J56" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="330">
+      <c r="A57" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B57" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C57" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="H57" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="150">
+      <c r="A58" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B58" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C58" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="J58" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="75">
+      <c r="A59" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B59" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C59" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="J59" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="105">
+      <c r="A60" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B60" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C60" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="J60" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="45">
+      <c r="A61" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B61" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C61" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="J61" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="120">
+      <c r="A62" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B62" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C62" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="I62" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="J62" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="225">
+      <c r="A63" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B63" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C63" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="J63" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="105">
+      <c r="A64" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B64" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C64" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="H64" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="J64" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="165">
+      <c r="A65" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B65" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C65" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="H65" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="J65" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="45">
+      <c r="A66" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B66" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C66" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="J66" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>